<commit_message>
fix excels as examples
</commit_message>
<xml_diff>
--- a/examples/excel_templates/course-credential.xlsx
+++ b/examples/excel_templates/course-credential.xlsx
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t xml:space="preserve">Haskell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
   </si>
 </sst>
 </file>
@@ -431,20 +434,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,8 +474,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -482,70 +489,70 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="19.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -562,7 +569,7 @@
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>44622</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -576,6 +583,12 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>